<commit_message>
corrected spelling error in cybersecurity requirements per taxonomy workbook
</commit_message>
<xml_diff>
--- a/source/reference_documents/working_material/cybersecurity requirements per taxonomy.xlsx
+++ b/source/reference_documents/working_material/cybersecurity requirements per taxonomy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.wilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F00B508-F9A3-2843-9929-29C8F049B64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C6B5A-9B45-0743-947F-AFA0939E578E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23420" yWindow="5500" windowWidth="23320" windowHeight="28160" xr2:uid="{56895247-3B3D-3147-A316-D5FB82A09ACE}"/>
+    <workbookView xWindow="50660" yWindow="2120" windowWidth="23320" windowHeight="28160" activeTab="1" xr2:uid="{56895247-3B3D-3147-A316-D5FB82A09ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="layer-asset-property sort" sheetId="5" r:id="rId1"/>
@@ -223,9 +223,6 @@
     <t>Configuration data confidentiality shall be protected using access controls.</t>
   </si>
   <si>
-    <t>Configuration data shall only be accessed by authenticate entities.</t>
-  </si>
-  <si>
     <t>Configuration data authenticity shall be assured.</t>
   </si>
   <si>
@@ -494,6 +491,9 @@
   </si>
   <si>
     <t>CR063</t>
+  </si>
+  <si>
+    <t>Configuration data shall only be accessed by authenticated entities.</t>
   </si>
 </sst>
 </file>
@@ -607,9 +607,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,7 +647,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -753,7 +753,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -895,7 +895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,9 +905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C74873-220C-9F48-A83A-36F8D7B5B9A6}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,7 +921,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
@@ -1058,7 +1058,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>56</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1438,10 +1438,10 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
         <v>61</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
         <v>60</v>
@@ -1566,10 +1566,10 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -1641,10 +1641,10 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
@@ -1666,10 +1666,10 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>46</v>
@@ -1694,10 +1694,10 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -1744,10 +1744,10 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
@@ -1769,10 +1769,10 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
@@ -1794,10 +1794,10 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="7"/>
@@ -1819,10 +1819,10 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
         <v>31</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
         <v>42</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
         <v>30</v>
@@ -2172,10 +2172,10 @@
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
         <v>28</v>
@@ -2223,10 +2223,10 @@
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="7" t="s">
@@ -2249,10 +2249,10 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>46</v>
@@ -2277,10 +2277,10 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>46</v>
@@ -2305,10 +2305,10 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>46</v>
@@ -2333,10 +2333,10 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>46</v>
@@ -2361,10 +2361,10 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="7" t="s">
@@ -2389,10 +2389,10 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58" s="6"/>
       <c r="E58" s="7"/>
@@ -2444,10 +2444,10 @@
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
@@ -2469,10 +2469,10 @@
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>46</v>
@@ -2519,10 +2519,10 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>46</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" t="s">
         <v>36</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
@@ -2650,9 +2650,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B3DCEF-5D6A-B948-BE1C-1FE631050A9D}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2666,7 +2666,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
@@ -2767,10 +2767,10 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
@@ -2803,7 +2803,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>56</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
@@ -3135,7 +3135,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -3183,10 +3183,10 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
         <v>61</v>
@@ -3286,7 +3286,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
         <v>60</v>
@@ -3311,10 +3311,10 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -3336,10 +3336,10 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -3361,10 +3361,10 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -3386,10 +3386,10 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
@@ -3411,10 +3411,10 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>46</v>
@@ -3439,10 +3439,10 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -3489,10 +3489,10 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
@@ -3514,10 +3514,10 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
@@ -3539,10 +3539,10 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>46</v>
@@ -3567,10 +3567,10 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
@@ -3592,10 +3592,10 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="7"/>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
         <v>44</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
         <v>33</v>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
@@ -3795,7 +3795,7 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -3845,10 +3845,10 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
         <v>42</v>
@@ -3895,10 +3895,10 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
         <v>30</v>
@@ -3945,10 +3945,10 @@
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>46</v>
@@ -3973,10 +3973,10 @@
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
@@ -3998,10 +3998,10 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>46</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>46</v>
@@ -4054,10 +4054,10 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>46</v>
@@ -4079,10 +4079,10 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="7" t="s">
@@ -4107,10 +4107,10 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
@@ -4135,10 +4135,10 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
@@ -4160,10 +4160,10 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58" s="6"/>
       <c r="E58" s="7"/>
@@ -4187,10 +4187,10 @@
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" t="s">
         <v>28</v>
@@ -4238,10 +4238,10 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="7" t="s">
@@ -4264,10 +4264,10 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>46</v>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" t="s">
         <v>36</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>

</xml_diff>